<commit_message>
Update retry sending mail if error occur
</commit_message>
<xml_diff>
--- a/templates/check-day.xlsx
+++ b/templates/check-day.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\172.16.1.217\~\drawing-file-automation\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B884C0F8-95D4-44EB-BB26-1FCAB220D5C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DF762A-A649-4740-8433-3B4E9D5E16CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -294,70 +294,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -678,10 +615,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
+      <selection pane="bottomLeft" activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -699,8 +636,10 @@
     <col min="15" max="18" width="7.7109375" style="3" customWidth="1"/>
     <col min="19" max="19" width="45.7109375" style="1" customWidth="1"/>
     <col min="20" max="20" width="7.7109375" style="1" customWidth="1"/>
-    <col min="21" max="22" width="15.7109375" style="1" customWidth="1"/>
-    <col min="23" max="25" width="15.7109375" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="8.28515625" style="1" customWidth="1"/>
+    <col min="23" max="24" width="8.28515625" customWidth="1"/>
+    <col min="25" max="25" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="24" x14ac:dyDescent="0.25">
@@ -808,15 +747,15 @@
       <c r="Y2" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="Y1:Y2">
-    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="VNTEC">
+  <conditionalFormatting sqref="Y1:Y1048576">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="VNTEC">
       <formula>NOT(ISERROR(SEARCH("VNTEC",Y1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="VT">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="VnTec">
+      <formula>NOT(ISERROR(SEARCH("VnTec",Y1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="VT">
       <formula>NOT(ISERROR(SEARCH("VT",Y1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="VnTec">
-      <formula>NOT(ISERROR(SEARCH("VnTec",Y1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>